<commit_message>
modified makeup class schedule
</commit_message>
<xml_diff>
--- a/FALL 19/makeup_class_track.xlsx
+++ b/FALL 19/makeup_class_track.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Course Code</t>
   </si>
@@ -60,13 +60,19 @@
     <t>Makeup classes taken on October 31</t>
   </si>
   <si>
-    <t>Makeup classes taken on December 12</t>
-  </si>
-  <si>
     <t>Makeup classes taken on December 19</t>
   </si>
   <si>
     <t>Makeup classes taken on December 26</t>
+  </si>
+  <si>
+    <t>Makeup classes taken on December 5</t>
+  </si>
+  <si>
+    <t>Makeup classes taken on January 2</t>
+  </si>
+  <si>
+    <t>Makeup classes taken on January 9</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -423,12 +429,14 @@
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="20.5703125" customWidth="1"/>
     <col min="10" max="10" width="33.42578125" customWidth="1"/>
-    <col min="11" max="12" width="34.7109375" customWidth="1"/>
+    <col min="11" max="11" width="33.7109375" customWidth="1"/>
+    <col min="12" max="12" width="34.7109375" customWidth="1"/>
     <col min="13" max="13" width="35.28515625" customWidth="1"/>
-    <col min="14" max="14" width="24.42578125" customWidth="1"/>
+    <col min="14" max="15" width="31.5703125" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1">
+    <row r="1" spans="1:16" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,19 +468,25 @@
         <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -489,18 +503,18 @@
         <f>C2+D2+E2+F2+G2+H2</f>
         <v>2</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
       <c r="N2">
-        <f>I2-J2-K2-L2-M2</f>
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <f>I2-J2-K2-L2-M2-N2-O2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -514,21 +528,21 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I7" si="0">C3+D3+E3+F3+G3+H3</f>
+        <f>C3+D3+E3+F3+G3+H3</f>
         <v>2</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
       <c r="N3">
-        <f t="shared" ref="N3:N7" si="1">I3-J3-K3-L3-M3</f>
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P7" si="0">I3-J3-K3-L3-M3-N3-O3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -545,24 +559,24 @@
         <v>1</v>
       </c>
       <c r="I4">
+        <f>C4+D4+E4+F4+G4+H4</f>
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="P4">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -572,59 +586,47 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
+        <f>C5+D5+E5+F5+G5+H5</f>
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
+        <f>C6+D6+E6+F6+G6+H6</f>
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -637,24 +639,18 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
       <c r="I7">
+        <f>C7+D7+E7+F7+G7+H7</f>
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified makeup class track and schedule
</commit_message>
<xml_diff>
--- a/FALL 19/makeup_class_track.xlsx
+++ b/FALL 19/makeup_class_track.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Course Code</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Makeup classes taken on January 2</t>
-  </si>
-  <si>
-    <t>Makeup classes taken on January 9</t>
   </si>
 </sst>
 </file>
@@ -414,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -432,11 +429,11 @@
     <col min="11" max="11" width="33.7109375" customWidth="1"/>
     <col min="12" max="12" width="34.7109375" customWidth="1"/>
     <col min="13" max="13" width="35.28515625" customWidth="1"/>
-    <col min="14" max="15" width="31.5703125" customWidth="1"/>
-    <col min="16" max="16" width="24.42578125" customWidth="1"/>
+    <col min="14" max="14" width="31.5703125" customWidth="1"/>
+    <col min="15" max="15" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1">
+    <row r="1" spans="1:15" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,13 +477,10 @@
         <v>17</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -500,21 +494,18 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <f>C2+D2+E2+F2+G2+H2</f>
+        <f t="shared" ref="I2:I7" si="0">C2+D2+E2+F2+G2+H2</f>
         <v>2</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <f>I2-J2-K2-L2-M2-N2-O2</f>
+        <f>I2-J2-K2-L2-M2-N2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -528,21 +519,18 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f>C3+D3+E3+F3+G3+H3</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P7" si="0">I3-J3-K3-L3-M3-N3-O3</f>
+        <f t="shared" ref="O3:O7" si="1">I3-J3-K3-L3-M3-N3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -559,7 +547,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <f>C4+D4+E4+F4+G4+H4</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K4">
@@ -571,12 +559,12 @@
       <c r="M4">
         <v>1</v>
       </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
+      <c r="O4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -586,47 +574,41 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
       <c r="I5">
-        <f>C5+D5+E5+F5+G5+H5</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
+      <c r="O5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="H6">
+      <c r="G6">
         <v>1</v>
       </c>
       <c r="I6">
-        <f>C6+D6+E6+F6+G6+H6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
+      <c r="O6">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -636,21 +618,15 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
       <c r="I7">
-        <f>C7+D7+E7+F7+G7+H7</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
+      <c r="O7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>